<commit_message>
Estrategia de Vendas Ponto Maximo
</commit_message>
<xml_diff>
--- a/Vendas.xlsx
+++ b/Vendas.xlsx
@@ -25,7 +25,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4125" uniqueCount="546">
   <si>
-    <t xml:space="preserve">ID-Produto</t>
+    <t xml:space="preserve">IDProduto</t>
   </si>
   <si>
     <t xml:space="preserve">Produto</t>
@@ -52,10 +52,10 @@
     <t xml:space="preserve">Vendedor</t>
   </si>
   <si>
-    <t xml:space="preserve">ID-Vendedor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data Venda</t>
+    <t xml:space="preserve">IDVendedor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DataVenda</t>
   </si>
   <si>
     <t xml:space="preserve">ValorVenda</t>
@@ -1771,8 +1771,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -1871,7 +1871,7 @@
   <dimension ref="A1:L458"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="122" zoomScaleNormal="122" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.3359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1890,7 +1890,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.66"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>